<commit_message>
adjusting minor parameters of multiple plots
</commit_message>
<xml_diff>
--- a/Figure_6/input/Colouring_tab.xlsx
+++ b/Figure_6/input/Colouring_tab.xlsx
@@ -91,7 +91,7 @@
     <t xml:space="preserve">untreated</t>
   </si>
   <si>
-    <t xml:space="preserve">Aci110</t>
+    <t xml:space="preserve">Aci 110</t>
   </si>
   <si>
     <t xml:space="preserve">wt</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">H^R</t>
   </si>
   <si>
-    <t xml:space="preserve">Aci110-1</t>
+    <t xml:space="preserve">A110-1</t>
   </si>
   <si>
     <t xml:space="preserve">H&lt;sup&gt;R&lt;/sup&gt;</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">HS^R</t>
   </si>
   <si>
-    <t xml:space="preserve">Aci110-2</t>
+    <t xml:space="preserve">A110-2</t>
   </si>
   <si>
     <t xml:space="preserve">HS&lt;sup&gt;R&lt;/sup&gt;</t>
@@ -226,7 +226,7 @@
     <t xml:space="preserve">HSFPh^R</t>
   </si>
   <si>
-    <t xml:space="preserve">Aci110-G1</t>
+    <t xml:space="preserve">A110-G1</t>
   </si>
   <si>
     <t xml:space="preserve">HSFPh&lt;sup&gt;R&lt;/sup&gt;</t>
@@ -578,27 +578,27 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q20" activeCellId="0" sqref="Q20"/>
+      <selection pane="bottomRight" activeCell="Q2" activeCellId="0" sqref="Q2:Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="18.97"/>

</xml_diff>